<commit_message>
Radiation shield BOM update
</commit_message>
<xml_diff>
--- a/hardware/Air & Light Sensors/BOM/BOM.xlsx
+++ b/hardware/Air & Light Sensors/BOM/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Desktop\Uni\5th year\Semester 2\Project\GitHub Folder\WeirWeather-AWS\hardware\Air &amp; Light Sensors\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87840F5C-18E7-49A3-A022-22D7172E972F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488EC95C-6AB9-4DD9-A10D-A9212BA30F55}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="19065" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BillOfMaterials" sheetId="2" r:id="rId1"/>
@@ -19,9 +19,9 @@
     <sheet name="©" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BillOfMaterials!$A$10:$E$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BillOfMaterials!$A$10:$G$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Example!$A$10:$H$10</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$H$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BillOfMaterials!$A$1:$J$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">Example!$A$1:$J$31</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">BillOfMaterials!$10:$10</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Example!$10:$10</definedName>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="104">
   <si>
     <t>[42]</t>
   </si>
@@ -337,20 +337,72 @@
     <t>M5 washer</t>
   </si>
   <si>
-    <t>Assembly Name : Radiation Shield</t>
-  </si>
-  <si>
-    <t>Part Count : 32.8</t>
-  </si>
-  <si>
-    <t>Total Cost : £ 34.57</t>
+    <t>Radiation Shield</t>
+  </si>
+  <si>
+    <t>Part Count :</t>
+  </si>
+  <si>
+    <t>Supplier2</t>
+  </si>
+  <si>
+    <t>Part No.</t>
+  </si>
+  <si>
+    <t>MOUSER</t>
+  </si>
+  <si>
+    <t>595-TMP117AIYBGR</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>125-1190</t>
+  </si>
+  <si>
+    <t>698-3324</t>
+  </si>
+  <si>
+    <t>432-450</t>
+  </si>
+  <si>
+    <t>FARNELL</t>
+  </si>
+  <si>
+    <t>403-SHT35-DIS-F</t>
+  </si>
+  <si>
+    <t>133-1672</t>
+  </si>
+  <si>
+    <t>814-9440</t>
+  </si>
+  <si>
+    <t>648-0935</t>
+  </si>
+  <si>
+    <t>743-2350</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>3DGBIRE</t>
+  </si>
+  <si>
+    <t>eBay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="7">
+    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
@@ -677,7 +729,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -843,13 +895,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="8" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="50">
+  <dxfs count="54">
     <dxf>
       <font>
         <b val="0"/>
@@ -998,6 +1051,32 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1061,56 +1140,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="169" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1134,6 +1164,7 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Trebuchet MS"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1143,7 +1174,7 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1159,88 +1190,17 @@
         <sz val="10"/>
         <color auto="1"/>
         <name val="Trebuchet MS"/>
+        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Trebuchet MS"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1827,6 +1787,201 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="169" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Trebuchet MS"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="55"/>
@@ -1966,16 +2121,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>354542</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>325967</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>372533</xdr:rowOff>
+      <xdr:rowOff>391583</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>526724</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>137376</xdr:rowOff>
+      <xdr:rowOff>156426</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1998,8 +2153,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2919942" y="372533"/>
-          <a:ext cx="2621165" cy="1525910"/>
+          <a:off x="4126442" y="391583"/>
+          <a:ext cx="2620107" cy="1650793"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2010,13 +2165,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1428750</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>321469</xdr:rowOff>
@@ -2060,13 +2215,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>2815</xdr:rowOff>
@@ -3273,16 +3428,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:H28" totalsRowCount="1" headerRowDxfId="49" dataDxfId="48" tableBorderDxfId="47">
-  <tableColumns count="8">
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="15" totalsRowDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Revision" dataDxfId="13" totalsRowDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="12" totalsRowDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="11" totalsRowDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Supplier" dataDxfId="10" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="9" totalsRowDxfId="1" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="8" totalsRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A10:J28" totalsRowCount="1" headerRowDxfId="53" dataDxfId="52" tableBorderDxfId="51">
+  <tableColumns count="10">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Part #" dataDxfId="50" totalsRowDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="49" totalsRowDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Revision" dataDxfId="48" totalsRowDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="47" totalsRowDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{98562C7E-8164-4D0B-8183-F33F8AB22546}" name="Supplier" dataDxfId="10" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{6F0151CA-8FEB-46D9-BADE-6E9BDCCE337B}" name="Part No." dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Units" dataDxfId="46" totalsRowDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Supplier2" dataDxfId="45" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Unit Cost" dataDxfId="44" totalsRowDxfId="1" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="43" totalsRowDxfId="0">
       <calculatedColumnFormula>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3291,29 +3448,29 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43" totalsRowBorderDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A6:C26" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Revision" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Revision Summary" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Approval Date" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="38" dataDxfId="37" tableBorderDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A10:J31" totalsRowCount="1" headerRowDxfId="34" dataDxfId="33" tableBorderDxfId="32">
   <tableColumns count="10">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="19" totalsRowDxfId="18" dataCellStyle="Currency"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="17" totalsRowDxfId="16">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Category" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Part #" dataDxfId="29" totalsRowDxfId="28"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Elem ID" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Part Name" totalsRowLabel="Total" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0200-00000A000000}" name="Color" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Qty" totalsRowFunction="sum" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Units" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="Picture" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Unit Cost" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Cost" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="12">
       <calculatedColumnFormula>Table14[[#This Row],[Qty]]*Table14[[#This Row],[Unit Cost]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3551,10 +3708,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -3562,19 +3719,20 @@
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="2" width="25.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.625" style="2" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="8.125" customWidth="1"/>
-    <col min="5" max="5" width="6.375" customWidth="1"/>
-    <col min="6" max="6" width="13.5" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="8" width="8.625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="22.625" customWidth="1"/>
-    <col min="11" max="11" width="10.125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.375" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="8.875" style="2"/>
+    <col min="4" max="5" width="8.125" customWidth="1"/>
+    <col min="6" max="6" width="16.375" customWidth="1"/>
+    <col min="7" max="7" width="6.375" customWidth="1"/>
+    <col min="8" max="8" width="13.5" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="8.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="22.625" customWidth="1"/>
+    <col min="13" max="13" width="10.125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="14.375" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="54" t="s">
         <v>66</v>
       </c>
@@ -3584,99 +3742,125 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="J2" s="5" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="2"/>
+      <c r="L2" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="J3" s="7" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="2"/>
+      <c r="L3" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="37" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="14"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="G4" s="2"/>
-      <c r="J4" s="2"/>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="37" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="14"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5">
+        <v>1</v>
+      </c>
       <c r="G5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="37" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="1"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H6" s="2"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>32.799999999999997</v>
+      </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="2"/>
+      <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H7" s="2"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" s="41" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="D8" s="63">
+        <v>34.57</v>
+      </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="2"/>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="H8" s="2"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="J9" s="2"/>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="2"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
@@ -3690,20 +3874,26 @@
         <v>11</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="9" t="s">
+      <c r="H10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="I10" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="J10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="55">
         <v>1</v>
       </c>
@@ -3715,19 +3905,25 @@
         <v>1</v>
       </c>
       <c r="E11" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="57">
+      <c r="H11" s="8"/>
+      <c r="I11" s="57">
         <v>5.96</v>
       </c>
-      <c r="H11" s="59">
+      <c r="J11" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>5.96</v>
       </c>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="55">
         <f>A11+1</f>
         <v>2</v>
@@ -3740,19 +3936,25 @@
         <v>2</v>
       </c>
       <c r="E12" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="57">
+      <c r="H12" s="8"/>
+      <c r="I12" s="57">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="H12" s="59">
+      <c r="J12" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>2.5999999999999999E-2</v>
       </c>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="55">
         <f t="shared" ref="A13:A22" si="0">A12+1</f>
         <v>3</v>
@@ -3765,19 +3967,25 @@
         <v>6</v>
       </c>
       <c r="E13" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>92</v>
+      </c>
+      <c r="G13" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="57">
+      <c r="H13" s="8"/>
+      <c r="I13" s="57">
         <v>0.05</v>
       </c>
-      <c r="H13" s="59">
+      <c r="J13" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="55">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3790,19 +3998,25 @@
         <v>7</v>
       </c>
       <c r="E14" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="56" t="s">
+        <v>93</v>
+      </c>
+      <c r="G14" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="57">
+      <c r="H14" s="8"/>
+      <c r="I14" s="57">
         <v>0.01</v>
       </c>
-      <c r="H14" s="59">
+      <c r="J14" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="J14" s="2"/>
-    </row>
-    <row r="15" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="55">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3815,19 +4029,25 @@
         <v>1</v>
       </c>
       <c r="E15" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" s="56">
+        <v>2709842</v>
+      </c>
+      <c r="G15" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="57">
+      <c r="H15" s="8"/>
+      <c r="I15" s="57">
         <v>1.72</v>
       </c>
-      <c r="H15" s="59">
+      <c r="J15" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>1.72</v>
       </c>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="55">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3840,19 +4060,25 @@
         <v>1</v>
       </c>
       <c r="E16" s="56" t="s">
+        <v>88</v>
+      </c>
+      <c r="F16" s="56" t="s">
+        <v>95</v>
+      </c>
+      <c r="G16" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="57">
+      <c r="H16" s="8"/>
+      <c r="I16" s="57">
         <v>8.24</v>
       </c>
-      <c r="H16" s="59">
+      <c r="J16" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>8.24</v>
       </c>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="55">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3865,19 +4091,25 @@
         <v>1</v>
       </c>
       <c r="E17" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="57">
+      <c r="H17" s="8"/>
+      <c r="I17" s="57">
         <v>1.1499999999999999</v>
       </c>
-      <c r="H17" s="59">
+      <c r="J17" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>1.1499999999999999</v>
       </c>
-      <c r="J17" s="2"/>
-    </row>
-    <row r="18" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="55">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3890,19 +4122,25 @@
         <v>1</v>
       </c>
       <c r="E18" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F18" s="56" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="57">
+      <c r="H18" s="8"/>
+      <c r="I18" s="57">
         <v>0.17</v>
       </c>
-      <c r="H18" s="59">
+      <c r="J18" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.17</v>
       </c>
-      <c r="J18" s="2"/>
-    </row>
-    <row r="19" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="55">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3915,19 +4153,25 @@
         <v>2</v>
       </c>
       <c r="E19" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="56" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="57">
+      <c r="H19" s="8"/>
+      <c r="I19" s="57">
         <v>0.04</v>
       </c>
-      <c r="H19" s="59">
+      <c r="J19" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.08</v>
       </c>
-      <c r="J19" s="2"/>
-    </row>
-    <row r="20" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="55">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3940,19 +4184,25 @@
         <v>1</v>
       </c>
       <c r="E20" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="8"/>
-      <c r="G20" s="57">
+      <c r="H20" s="8"/>
+      <c r="I20" s="57">
         <v>0.5</v>
       </c>
-      <c r="H20" s="59">
+      <c r="J20" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.5</v>
       </c>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="55">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3965,19 +4215,25 @@
         <v>1</v>
       </c>
       <c r="E21" s="56" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="56">
+        <v>7482280</v>
+      </c>
+      <c r="G21" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="8"/>
-      <c r="G21" s="57">
+      <c r="H21" s="8"/>
+      <c r="I21" s="57">
         <v>1.89</v>
       </c>
-      <c r="H21" s="59">
+      <c r="J21" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>1.89</v>
       </c>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="22" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="55">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3990,19 +4246,25 @@
         <v>1</v>
       </c>
       <c r="E22" s="56" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="8"/>
-      <c r="G22" s="57">
+      <c r="H22" s="8"/>
+      <c r="I22" s="57">
         <v>3.06</v>
       </c>
-      <c r="H22" s="59">
+      <c r="J22" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>3.06</v>
       </c>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="55">
         <f>A22+1</f>
         <v>13</v>
@@ -4015,19 +4277,25 @@
         <v>0.3</v>
       </c>
       <c r="E23" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="F23" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F23" s="8"/>
-      <c r="G23" s="57">
+      <c r="H23" s="8"/>
+      <c r="I23" s="57">
         <v>24</v>
       </c>
-      <c r="H23" s="59">
+      <c r="J23" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>7.1999999999999993</v>
       </c>
-      <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="55">
         <v>14</v>
       </c>
@@ -4039,19 +4307,25 @@
         <v>0.5</v>
       </c>
       <c r="E24" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="57">
+      <c r="H24" s="8"/>
+      <c r="I24" s="57">
         <v>6.37</v>
       </c>
-      <c r="H24" s="59">
+      <c r="J24" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>3.1850000000000001</v>
       </c>
-      <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="55">
         <v>15</v>
       </c>
@@ -4063,19 +4337,25 @@
         <v>3</v>
       </c>
       <c r="E25" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="8"/>
-      <c r="G25" s="57">
+      <c r="H25" s="8"/>
+      <c r="I25" s="57">
         <v>0.18</v>
       </c>
-      <c r="H25" s="59">
+      <c r="J25" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.54</v>
       </c>
-      <c r="J25" s="2"/>
-    </row>
-    <row r="26" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="55">
         <v>16</v>
       </c>
@@ -4087,19 +4367,25 @@
         <v>1</v>
       </c>
       <c r="E26" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G26" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F26" s="8"/>
-      <c r="G26" s="57">
+      <c r="H26" s="8"/>
+      <c r="I26" s="57">
         <v>0.18</v>
       </c>
-      <c r="H26" s="59">
+      <c r="J26" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.18</v>
       </c>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="55">
         <v>17</v>
       </c>
@@ -4111,19 +4397,25 @@
         <v>3</v>
       </c>
       <c r="E27" s="56" t="s">
+        <v>103</v>
+      </c>
+      <c r="F27" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="56" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="8"/>
-      <c r="G27" s="57">
+      <c r="H27" s="8"/>
+      <c r="I27" s="57">
         <v>0.1</v>
       </c>
-      <c r="H27" s="59">
+      <c r="J27" s="59">
         <f>Table1[[#This Row],[Qty]]*Table1[[#This Row],[Unit Cost]]</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="J27" s="2"/>
-    </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.3">
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="1:12" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="11"/>
       <c r="B28" s="11" t="s">
         <v>8</v>
@@ -4134,60 +4426,86 @@
         <v>32.799999999999997</v>
       </c>
       <c r="E28" s="12"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="18"/>
-      <c r="H28" s="58">
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="58">
         <f>SUBTOTAL(109,Table1[Cost])</f>
         <v>34.570999999999998</v>
       </c>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D29" s="2"/>
-      <c r="J29" s="2"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D30" s="2"/>
-      <c r="J30" s="2"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D31" s="2"/>
-      <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D32" s="2"/>
-      <c r="J32" s="2"/>
-    </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
-      <c r="J33" s="2"/>
-    </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D34" s="2"/>
-    </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D35" s="2"/>
-    </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D36" s="2"/>
-    </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D37" s="2"/>
-    </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D38" s="2"/>
-    </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D39" s="2"/>
-    </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="4:12" x14ac:dyDescent="0.3">
       <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://www.vertex42.com/ExcelTemplates/free-timesheet-template.html" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="J3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.5" footer="0.5"/>

</xml_diff>